<commit_message>
saving and loadin in booked guests implemented
</commit_message>
<xml_diff>
--- a/main/src/main/resources/guests_state.xlsx
+++ b/main/src/main/resources/guests_state.xlsx
@@ -12,18 +12,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
-    <t>pppp</t>
+    <t>Peter</t>
   </si>
   <si>
-    <t>ppppppppppp</t>
+    <t>Donat</t>
   </si>
   <si>
-    <t>2024-11-25</t>
+    <t>2024-11-18</t>
   </si>
   <si>
-    <t>2024-11-30</t>
+    <t>2024-11-20</t>
+  </si>
+  <si>
+    <t>Gregory</t>
+  </si>
+  <si>
+    <t>Mosh</t>
+  </si>
+  <si>
+    <t>mario</t>
+  </si>
+  <si>
+    <t>cart</t>
   </si>
 </sst>
 </file>
@@ -68,7 +80,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -85,7 +97,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="n" s="0">
-        <v>1.0</v>
+        <v>123.0</v>
       </c>
       <c r="E1" t="s" s="0">
         <v>2</v>
@@ -94,6 +106,46 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n" s="0">
+        <v>101.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>456.0</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>102.0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>111.0</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
sonarqube with jacoco included
</commit_message>
<xml_diff>
--- a/main/src/main/resources/guests_state.xlsx
+++ b/main/src/main/resources/guests_state.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Peter</t>
   </si>
@@ -35,7 +35,13 @@
     <t>mario</t>
   </si>
   <si>
-    <t>cart</t>
+    <t>donat</t>
+  </si>
+  <si>
+    <t>2024-11-23</t>
+  </si>
+  <si>
+    <t>anette</t>
   </si>
 </sst>
 </file>
@@ -80,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -137,13 +143,33 @@
         <v>7</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>111.0</v>
+        <v>11111.0</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>2</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>3</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>102.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>22333.0</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more rooms added in default version
</commit_message>
<xml_diff>
--- a/main/src/main/resources/guests_state.xlsx
+++ b/main/src/main/resources/guests_state.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>Donat</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Berry</t>
   </si>
   <si>
     <t>2024-11-18</t>
@@ -26,22 +26,34 @@
     <t>2024-11-20</t>
   </si>
   <si>
-    <t>Gregory</t>
-  </si>
-  <si>
-    <t>Mosh</t>
-  </si>
-  <si>
-    <t>mario</t>
-  </si>
-  <si>
-    <t>donat</t>
-  </si>
-  <si>
-    <t>2024-11-23</t>
-  </si>
-  <si>
-    <t>anette</t>
+    <t>Julie</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Maklowicz</t>
+  </si>
+  <si>
+    <t>2024-11-19</t>
+  </si>
+  <si>
+    <t>2024-11-30</t>
+  </si>
+  <si>
+    <t>Connor</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>2024-11-25</t>
+  </si>
+  <si>
+    <t>Amanda</t>
+  </si>
+  <si>
+    <t>Carol</t>
   </si>
 </sst>
 </file>
@@ -86,7 +98,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -103,7 +115,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="n" s="0">
-        <v>123.0</v>
+        <v>182745.0</v>
       </c>
       <c r="E1" t="s" s="0">
         <v>2</v>
@@ -120,10 +132,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>456.0</v>
+        <v>283746.0</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>2</v>
@@ -137,16 +149,16 @@
         <v>102.0</v>
       </c>
       <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>7</v>
-      </c>
       <c r="D3" t="n" s="0">
-        <v>11111.0</v>
+        <v>123456.0</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s" s="0">
         <v>8</v>
@@ -154,22 +166,62 @@
     </row>
     <row r="4">
       <c r="A4" t="n" s="0">
-        <v>102.0</v>
+        <v>105.0</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>9</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>22333.0</v>
+        <v>273646.0</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>8</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>105.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>374746.0</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>105.0</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <v>283665.0</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>